<commit_message>
Metrics plotting and selection.
</commit_message>
<xml_diff>
--- a/data/metrics/june2021_rerun/sens.filt_seed60_2021-06-14.xlsx
+++ b/data/metrics/june2021_rerun/sens.filt_seed60_2021-06-14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LGSS_scripting\lgss\data\metrics\june2021_rerun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F0B822-A204-4CA9-A664-A1A04426B938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9859F0A5-A1FB-424D-A905-D0ED7211925D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2090" yWindow="570" windowWidth="19400" windowHeight="11000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sens.filt_seed60_2021-06-14" sheetId="1" r:id="rId1"/>
@@ -725,12 +725,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -744,6 +742,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1101,14 +1102,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1121,7 +1122,7 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1150,10 +1151,10 @@
       <c r="B2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1301,7 +1302,7 @@
       <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1328,7 +1329,7 @@
       <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
@@ -1357,7 +1358,7 @@
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
@@ -1375,7 +1376,7 @@
       <c r="I9">
         <v>22.7</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="15">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1386,7 +1387,7 @@
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E10" t="s">
@@ -1404,7 +1405,7 @@
       <c r="I10">
         <v>7.6</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="11">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1415,7 +1416,7 @@
       <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
@@ -1433,7 +1434,7 @@
       <c r="I11">
         <v>7.6</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="12">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1505,7 +1506,7 @@
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1532,10 +1533,10 @@
       <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="4"/>
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1562,7 +1563,7 @@
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
@@ -1591,7 +1592,7 @@
       <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
@@ -1609,7 +1610,7 @@
       <c r="I17">
         <v>1.7388390811777801</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="9">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1620,7 +1621,7 @@
       <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E18" t="s">
@@ -1638,7 +1639,7 @@
       <c r="I18">
         <v>1.7388390811777801</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="13">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1649,7 +1650,7 @@
       <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E19" t="s">
@@ -1667,7 +1668,7 @@
       <c r="I19">
         <v>1.3585886750538401</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="13">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1678,7 +1679,7 @@
       <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E20" t="s">
@@ -1696,7 +1697,7 @@
       <c r="I20">
         <v>1.37481323095226</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="13">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1707,7 +1708,7 @@
       <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E21" t="s">
@@ -1725,7 +1726,7 @@
       <c r="I21">
         <v>2.0575240379824198</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="13">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1736,7 +1737,7 @@
       <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E22" t="s">
@@ -1754,7 +1755,7 @@
       <c r="I22">
         <v>2.0575240379824198</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="13">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1765,7 +1766,7 @@
       <c r="B23" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E23" t="s">
@@ -1783,7 +1784,7 @@
       <c r="I23">
         <v>1.7453848104163701</v>
       </c>
-      <c r="J23" s="16">
+      <c r="J23" s="14">
         <v>76.923076923076906</v>
       </c>
     </row>
@@ -1983,16 +1984,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>